<commit_message>
- Define mês e ano a partir dos argumentos na linha de comando - Determina os secrets automaticamente usando como seed o ano+mês - Problemas de encoding resolvidos
</commit_message>
<xml_diff>
--- a/input/maio_2016_compl.xlsx
+++ b/input/maio_2016_compl.xlsx
@@ -8,9 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Plan2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Plan3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="maio_2016_compl" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -73,13 +71,11 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="6">
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+  <fonts count="4">
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -95,20 +91,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="9.95"/>
-      <color rgb="FF000000"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="MS Sans Serif"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -128,7 +110,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -152,29 +134,20 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -190,128 +163,76 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.0647773279352"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.90816326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.4489795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="0" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="0" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="0" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="0" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
-  </cols>
-  <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
-  </cols>
-  <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>